<commit_message>
Nuuchahnulth: add burndown chart for tagging data
</commit_message>
<xml_diff>
--- a/data/reports/Nuuchahnulth data progress.xlsx
+++ b/data/reports/Nuuchahnulth data progress.xlsx
@@ -1,36 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/data/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="609" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79946DEC-6F31-4BAD-9531-4960533397F1}"/>
+  <xr:revisionPtr revIDLastSave="786" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E82302E-D7F1-4861-B494-DF427A0DBA5E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="4" r:id="rId1"/>
-    <sheet name="data" sheetId="5" r:id="rId2"/>
-    <sheet name="backend" sheetId="6" r:id="rId3"/>
+    <sheet name="typing" sheetId="5" r:id="rId2"/>
+    <sheet name="tagging" sheetId="7" r:id="rId3"/>
+    <sheet name="backend" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">tagging!$A$2:$A$13</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">tagging!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">tagging!$B$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">tagging!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">tagging!$C$2:$C$13</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">tagging!$A$2:$A$13</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">tagging!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">tagging!$B$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">tagging!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">tagging!$C$2:$C$13</definedName>
+    <definedName name="Auto_Tagged_Tokens">backend!$E$2</definedName>
     <definedName name="CL_Pages">backend!$B$9</definedName>
     <definedName name="CL_Start_Pages">backend!$B$6</definedName>
-    <definedName name="Current_Book">data!$B$3</definedName>
-    <definedName name="Current_Line">data!$B$2</definedName>
-    <definedName name="Current_Page">data!$B$4</definedName>
+    <definedName name="Current_Book">typing!$B$3</definedName>
+    <definedName name="Current_Line">typing!$B$2</definedName>
+    <definedName name="Current_Page">typing!$B$4</definedName>
     <definedName name="GL_Pages">backend!$B$8</definedName>
     <definedName name="GL_Start_Pages">backend!$B$5</definedName>
-    <definedName name="Line_Pages_Completed">data!$B$5</definedName>
-    <definedName name="Line_Pages_Remaining">data!$B$6</definedName>
+    <definedName name="Line_Pages_Completed">typing!$B$5</definedName>
+    <definedName name="Line_Pages_Remaining">typing!$B$6</definedName>
     <definedName name="Total_Line_Pages">backend!$B$11</definedName>
     <definedName name="Total_Pages">backend!$B$12</definedName>
-    <definedName name="Total_Pages_Completed">data!$B$7</definedName>
-    <definedName name="Total_Pages_Remaining">data!$B$8</definedName>
+    <definedName name="Total_Pages_Completed">typing!$B$7</definedName>
+    <definedName name="Total_Pages_Remaining">typing!$B$8</definedName>
+    <definedName name="Total_Tokens">backend!$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,8 +62,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Total Pages</t>
   </si>
@@ -132,12 +167,42 @@
   <si>
     <t>Burndown Log</t>
   </si>
+  <si>
+    <t>Target Words Tagged</t>
+  </si>
+  <si>
+    <t>Actual Words Tagged</t>
+  </si>
+  <si>
+    <t>Total Tokens</t>
+  </si>
+  <si>
+    <t>Auto Tagged Tokens</t>
+  </si>
+  <si>
+    <t>Daily Average to Hit</t>
+  </si>
+  <si>
+    <t>Tokens Remaining</t>
+  </si>
+  <si>
+    <t>% Done</t>
+  </si>
+  <si>
+    <t>Target Words Remaining</t>
+  </si>
+  <si>
+    <t>Actual Words Remaining</t>
+  </si>
+  <si>
+    <t>Words Remaining</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +244,19 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -425,14 +503,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -512,15 +591,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -550,15 +698,9 @@
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -569,7 +711,10 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -592,11 +737,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$10</c:f>
+              <c:f>tagging!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total Percentage Completed</c:v>
+                  <c:v>% Done</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -611,76 +756,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>data!$B$10</c:f>
+              <c:f>tagging!$H$2</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.37329667702605784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C714-4345-BC3F-78A80CC2A4F6}"/>
+              <c16:uniqueId val="{00000000-7A32-4CD5-9C76-7B9791365F74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -693,20 +783,54 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="638937647"/>
-        <c:axId val="556222351"/>
+        <c:axId val="166151455"/>
+        <c:axId val="212717503"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="638937647"/>
+        <c:axId val="166151455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="556222351"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="212717503"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -714,11 +838,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="556222351"/>
+        <c:axId val="212717503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -736,7 +859,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -767,7 +890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638937647"/>
+        <c:crossAx val="166151455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -781,13 +904,488 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Target vs. Actual Words Remaining</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tagging!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Target Words Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>tagging!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44076</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44086</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tagging!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4766.363636363636</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4289.727272727273</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3813.090909090909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3336.454545454546</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2859.818181818182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2383.181818181818</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1906.545454545454</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1429.909090909091</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>953.27272727272702</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>476.63636363636397</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B9C-4347-9C4E-058F566E09A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tagging!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Words Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>tagging!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44076</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44086</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tagging!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7B9C-4347-9C4E-058F566E09A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="316043039"/>
+        <c:axId val="179029311"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="316043039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="179029311"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="179029311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316043039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -863,6 +1461,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -1336,6 +1974,522 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1378,17 +2532,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443689D3-D351-47F9-A10D-1A97CE7D75FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6224341B-893E-44F6-868F-E33F9A9D2326}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1408,7 +2562,121 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4CBC3A4-118C-4617-B913-D983CB567906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F0DE02E-8409-48BA-B123-0B7DF2AFEA71}" name="Table3" displayName="Table3" ref="Q1:Q2" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="Q1:Q2" xr:uid="{AE6264B3-D76F-49E5-927B-4BBE73641000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{201E545C-0FB4-4BC7-946A-ECAF21C4B803}" name="Words Remaining" dataDxfId="5">
+      <calculatedColumnFormula>Table2[[#This Row],[Tokens Remaining]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AA23A943-CFE1-4A72-B03B-8CA47906371C}" name="Table4" displayName="Table4" ref="Q4:Q5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="Q4:Q5" xr:uid="{DC3D502B-0A69-4F88-8386-CCCB5C3DE5E5}">
+    <filterColumn colId="0" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B726FDFB-69DA-4847-BC09-948270FE4F9F}" name="Daily Average to Hit" dataDxfId="2">
+      <calculatedColumnFormula array="1">Table2[Daily Average to Hit]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00D94B6B-22EC-4315-A578-7EF3BDBFEF6E}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13" xr:uid="{695ACE7C-3E30-4362-BD96-BF7BE671C241}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2EDA5029-9539-49A0-8197-49D44DF6D198}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{9B85D289-D1D5-48F9-B2BF-A2D7778C94E3}" name="Target Words Tagged" dataDxfId="10">
+      <calculatedColumnFormula>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7FBAA802-6FAF-4A5E-AFFA-CA609751AC3A}" name="Actual Words Tagged" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{01DDBF48-FF6C-44B7-8F3F-804C348DF245}" name="Target Words Remaining" dataDxfId="7">
+      <calculatedColumnFormula>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{E19FADB1-29D3-4E29-9625-D495706317E6}" name="Actual Words Remaining" dataDxfId="6">
+      <calculatedColumnFormula>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68F2EC6B-0CC0-4C80-9BD4-7166E06A5FA8}" name="Table2" displayName="Table2" ref="G1:I2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="G1:I2" xr:uid="{626B0A7D-3289-4586-BF03-1693112A10A4}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{02FD5AFB-3956-4A8F-96BD-72889454C1E4}" name="Tokens Remaining" dataDxfId="15">
+      <calculatedColumnFormula>Total_Tokens - MAX(C2:C13)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{849E5411-18D7-4FCB-9D80-595D080B3C4B}" name="% Done" dataDxfId="8" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{76BBA636-7635-44DF-A536-1B32031FBBED}" name="Daily Average to Hit" dataDxfId="14">
+      <calculatedColumnFormula>G2/COUNTBLANK(C2:C13)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1708,16 +2976,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99EB4AA-F4ED-40DA-BCD9-5BEAE4C66053}">
-  <dimension ref="A1"/>
+  <dimension ref="Q1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="17" max="17" width="17" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="17:17" x14ac:dyDescent="0.45">
+      <c r="Q1" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="17:17" x14ac:dyDescent="0.45">
+      <c r="Q2" s="29">
+        <f>Table2[[#This Row],[Tokens Remaining]]</f>
+        <v>5243</v>
+      </c>
+    </row>
+    <row r="4" spans="17:17" x14ac:dyDescent="0.45">
+      <c r="Q4" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="17:17" x14ac:dyDescent="0.45">
+      <c r="Q5" s="30" cm="1">
+        <f t="array" ref="Q5">Table2[Daily Average to Hit]</f>
+        <v>476.63636363636363</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1725,7 +3023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84877C8-368F-4B94-AA14-70D81601CFC3}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2366,35 +3664,347 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4384D275-DAF3-4D61-8040-B7C860B54327}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4E6563-AFDF-481D-85FD-ACA04DEA8072}">
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.73046875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.06640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.9296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.9296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.9296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.9296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>44076</v>
+      </c>
+      <c r="B2" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>3123</v>
+      </c>
+      <c r="C2" s="30">
+        <v>3123</v>
+      </c>
+      <c r="D2" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>5243</v>
+      </c>
+      <c r="E2" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</f>
+        <v>5243</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="29">
+        <f>Total_Tokens - MAX(C2:C13)</f>
+        <v>5243</v>
+      </c>
+      <c r="H2" s="32">
+        <f>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</f>
+        <v>0.37329667702605784</v>
+      </c>
+      <c r="I2" s="30">
+        <f>G2/COUNTBLANK(C2:C13)</f>
+        <v>476.63636363636363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>44077</v>
+      </c>
+      <c r="B3" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>3599.6363636363635</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>4766.363636363636</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>44078</v>
+      </c>
+      <c r="B4" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>4076.272727272727</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>4289.727272727273</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>44079</v>
+      </c>
+      <c r="B5" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>4552.909090909091</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>3813.090909090909</v>
+      </c>
+      <c r="E5" s="30"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>44080</v>
+      </c>
+      <c r="B6" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>5029.545454545454</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>3336.454545454546</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>44081</v>
+      </c>
+      <c r="B7" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>5506.181818181818</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>2859.818181818182</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>44082</v>
+      </c>
+      <c r="B8" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>5982.818181818182</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>2383.181818181818</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>44083</v>
+      </c>
+      <c r="B9" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>6459.454545454546</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>1906.545454545454</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>44084</v>
+      </c>
+      <c r="B10" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>6936.090909090909</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>1429.909090909091</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B11" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>7412.727272727273</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>953.27272727272702</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>44086</v>
+      </c>
+      <c r="B12" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>7889.363636363636</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>476.63636363636397</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>44087</v>
+      </c>
+      <c r="B13" s="30">
+        <f>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</f>
+        <v>8366</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30">
+        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4384D275-DAF3-4D61-8040-B7C860B54327}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1">
+        <v>8366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2402,7 +4012,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2410,7 +4020,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2418,7 +4028,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2426,7 +4036,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2435,7 +4045,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add tags for English / nonsense words
</commit_message>
<xml_diff>
--- a/data/reports/Nuuchahnulth data progress.xlsx
+++ b/data/reports/Nuuchahnulth data progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/data/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="833" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BEEAAEC-6AA2-43E6-9672-D24FBAD90F1C}"/>
+  <xr:revisionPtr revIDLastSave="836" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33589806-3461-422B-BFF3-C8CA24C9BE5A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,9 @@
     <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,9 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
@@ -620,15 +620,6 @@
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -678,6 +669,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -793,7 +793,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.39660530719579251</c:v>
+                  <c:v>0.45266555103992351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,7 +1248,7 @@
                   <c:v>5243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5048</c:v>
+                  <c:v>4579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2665,12 +2665,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA40D1A7-8457-439D-9848-1C74FD453534}" name="Table5" displayName="Table5" ref="Q7:Q8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA40D1A7-8457-439D-9848-1C74FD453534}" name="Table5" displayName="Table5" ref="Q7:Q8" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="Q7:Q8" xr:uid="{97450FB2-4251-49FC-905A-8B7F73A3F6E2}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A9EA3493-B5C5-45C0-B2D0-2806806CEBAB}" name="Tagged Today" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{A9EA3493-B5C5-45C0-B2D0-2806806CEBAB}" name="Tagged Today" dataDxfId="11">
       <calculatedColumnFormula array="1">Table2[Tagged Today]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2688,15 +2688,15 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2EDA5029-9539-49A0-8197-49D44DF6D198}" name="Date" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{9B85D289-D1D5-48F9-B2BF-A2D7778C94E3}" name="Target Words Tagged" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{2EDA5029-9539-49A0-8197-49D44DF6D198}" name="Date" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{9B85D289-D1D5-48F9-B2BF-A2D7778C94E3}" name="Target Words Tagged" dataDxfId="9">
       <calculatedColumnFormula>((Total_Tokens-Auto_Tagged_Tokens)/11*(ROW()-2))+ Auto_Tagged_Tokens</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7FBAA802-6FAF-4A5E-AFFA-CA609751AC3A}" name="Actual Words Tagged" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{01DDBF48-FF6C-44B7-8F3F-804C348DF245}" name="Target Words Remaining" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{7FBAA802-6FAF-4A5E-AFFA-CA609751AC3A}" name="Actual Words Tagged" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{01DDBF48-FF6C-44B7-8F3F-804C348DF245}" name="Target Words Remaining" dataDxfId="7">
       <calculatedColumnFormula>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E19FADB1-29D3-4E29-9625-D495706317E6}" name="Actual Words Remaining" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{E19FADB1-29D3-4E29-9625-D495706317E6}" name="Actual Words Remaining" dataDxfId="6">
       <calculatedColumnFormula>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2705,7 +2705,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68F2EC6B-0CC0-4C80-9BD4-7166E06A5FA8}" name="Table2" displayName="Table2" ref="G1:J2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68F2EC6B-0CC0-4C80-9BD4-7166E06A5FA8}" name="Table2" displayName="Table2" ref="G1:J2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="G1:J2" xr:uid="{626B0A7D-3289-4586-BF03-1693112A10A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2713,16 +2713,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02FD5AFB-3956-4A8F-96BD-72889454C1E4}" name="Tokens Remaining" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{02FD5AFB-3956-4A8F-96BD-72889454C1E4}" name="Tokens Remaining" dataDxfId="3">
       <calculatedColumnFormula>Total_Tokens - MAX(C2:C13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{849E5411-18D7-4FCB-9D80-595D080B3C4B}" name="% Done" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{849E5411-18D7-4FCB-9D80-595D080B3C4B}" name="% Done" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{76BBA636-7635-44DF-A536-1B32031FBBED}" name="Daily Average to Hit" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{76BBA636-7635-44DF-A536-1B32031FBBED}" name="Daily Average to Hit" dataDxfId="1">
       <calculatedColumnFormula>G2/COUNTBLANK(C2:C13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C8777993-E2BD-4126-8780-8EF08387FFEE}" name="Tagged Today" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{C8777993-E2BD-4126-8780-8EF08387FFEE}" name="Tagged Today" dataDxfId="0">
       <calculatedColumnFormula array="1">LOOKUP(2,1/(Table1[Actual Words Tagged]&lt;&gt;""),Table1[Actual Words Tagged])-INDEX(Table1[Actual Words Tagged],MATCH(99^99,Table1[Actual Words Tagged],1)-1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3046,7 +3046,7 @@
     <row r="2" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q2" s="19">
         <f>Table2[[#This Row],[Tokens Remaining]]</f>
-        <v>5048</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="4" spans="17:17" x14ac:dyDescent="0.45">
@@ -3057,7 +3057,7 @@
     <row r="5" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q5" s="20" cm="1">
         <f t="array" ref="Q5">Table2[Daily Average to Hit]</f>
-        <v>504.8</v>
+        <v>457.9</v>
       </c>
     </row>
     <row r="7" spans="17:17" x14ac:dyDescent="0.45">
@@ -3068,7 +3068,7 @@
     <row r="8" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q8" s="19" cm="1">
         <f t="array" ref="Q8">Table2[Tagged Today]</f>
-        <v>195</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -3105,16 +3105,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="D1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
@@ -3149,7 +3149,7 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="1">
         <v>43807</v>
       </c>
@@ -3177,7 +3177,7 @@
       <c r="B4" s="2">
         <v>347</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="1">
         <v>43808</v>
       </c>
@@ -3205,7 +3205,7 @@
         <f>IF(Current_Book="GL",Current_Page-GL_Start_Pages,GL_Pages-GL_Start_Pages+Current_Page-CL_Start_Pages)</f>
         <v>747</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="1">
         <v>43809</v>
       </c>
@@ -3233,7 +3233,7 @@
         <f>Total_Line_Pages-Line_Pages_Completed</f>
         <v>0</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="1">
         <v>43810</v>
       </c>
@@ -3261,7 +3261,7 @@
         <f>(Total_Line_Pages*Current_Line)-Line_Pages_Remaining</f>
         <v>3735</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="1">
         <v>43811</v>
       </c>
@@ -3289,7 +3289,7 @@
         <f>(Total_Pages)-Total_Pages_Completed</f>
         <v>0</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="1">
         <v>43812</v>
       </c>
@@ -3317,7 +3317,7 @@
         <f>Line_Pages_Completed/Total_Line_Pages</f>
         <v>1</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="1">
         <v>43813</v>
       </c>
@@ -3345,7 +3345,7 @@
         <f>Total_Pages_Completed/(Total_Pages)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="1">
         <v>43814</v>
       </c>
@@ -3366,7 +3366,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D11" s="33"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="1">
         <v>43815</v>
       </c>
@@ -3387,7 +3387,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D12" s="33"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="1">
         <v>43816</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D13" s="33"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="1">
         <v>43817</v>
       </c>
@@ -3429,7 +3429,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D14" s="33"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="1">
         <v>43818</v>
       </c>
@@ -3450,7 +3450,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D15" s="33"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="1">
         <v>43819</v>
       </c>
@@ -3471,7 +3471,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="33" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="1">
@@ -3494,7 +3494,7 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D17" s="32"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="1">
         <v>43821</v>
       </c>
@@ -3515,7 +3515,7 @@
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D18" s="32"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="1">
         <v>43822</v>
       </c>
@@ -3536,7 +3536,7 @@
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="1">
         <v>43823</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D20" s="32"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="1">
         <v>43824</v>
       </c>
@@ -3578,7 +3578,7 @@
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D21" s="32"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="1">
         <v>43825</v>
       </c>
@@ -3599,7 +3599,7 @@
       </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D22" s="32"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="1">
         <v>43826</v>
       </c>
@@ -3620,7 +3620,7 @@
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D23" s="24"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="1">
         <v>43827</v>
       </c>
@@ -3641,7 +3641,7 @@
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D24" s="25"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="1">
         <v>43828</v>
       </c>
@@ -3662,7 +3662,7 @@
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D25" s="26"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="1">
         <v>43829</v>
       </c>
@@ -3731,7 +3731,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3790,7 +3790,6 @@
         <v>3123</v>
       </c>
       <c r="D2" s="20">
-        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
         <v>5243</v>
       </c>
       <c r="E2" s="20">
@@ -3800,19 +3799,19 @@
       <c r="F2" s="8"/>
       <c r="G2" s="19">
         <f>Total_Tokens - MAX(C2:C13)</f>
-        <v>5048</v>
+        <v>4579</v>
       </c>
       <c r="H2" s="22">
         <f>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</f>
-        <v>0.39660530719579251</v>
+        <v>0.45266555103992351</v>
       </c>
       <c r="I2" s="20">
         <f>G2/COUNTBLANK(C2:C13)</f>
-        <v>504.8</v>
-      </c>
-      <c r="J2" s="34" cm="1">
+        <v>457.9</v>
+      </c>
+      <c r="J2" s="24" cm="1">
         <f t="array" ref="J2">LOOKUP(2,1/(Table1[Actual Words Tagged]&lt;&gt;""),Table1[Actual Words Tagged])-INDEX(Table1[Actual Words Tagged],MATCH(99^99,Table1[Actual Words Tagged],1)-1)</f>
-        <v>195</v>
+        <v>664</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -3824,15 +3823,14 @@
         <v>3599.6363636363635</v>
       </c>
       <c r="C3" s="20">
-        <v>3318</v>
+        <v>3787</v>
       </c>
       <c r="D3" s="20">
-        <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
         <v>4766.363636363636</v>
       </c>
       <c r="E3" s="20">
         <f>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</f>
-        <v>5048</v>
+        <v>4579</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="6"/>

</xml_diff>

<commit_message>
add tags for complementizers
</commit_message>
<xml_diff>
--- a/data/reports/Nuuchahnulth data progress.xlsx
+++ b/data/reports/Nuuchahnulth data progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/data/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="836" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33589806-3461-422B-BFF3-C8CA24C9BE5A}"/>
+  <xr:revisionPtr revIDLastSave="838" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56E8AC53-DA68-4F6D-8576-427D6E57551D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="4" r:id="rId1"/>
@@ -793,7 +793,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.45266555103992351</c:v>
+                  <c:v>0.49737030839110685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,6 +1249,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4579</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3029,7 +3032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99EB4AA-F4ED-40DA-BCD9-5BEAE4C66053}">
   <dimension ref="Q1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -3046,7 +3049,7 @@
     <row r="2" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q2" s="19">
         <f>Table2[[#This Row],[Tokens Remaining]]</f>
-        <v>4579</v>
+        <v>4205</v>
       </c>
     </row>
     <row r="4" spans="17:17" x14ac:dyDescent="0.45">
@@ -3057,7 +3060,7 @@
     <row r="5" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q5" s="20" cm="1">
         <f t="array" ref="Q5">Table2[Daily Average to Hit]</f>
-        <v>457.9</v>
+        <v>467.22222222222223</v>
       </c>
     </row>
     <row r="7" spans="17:17" x14ac:dyDescent="0.45">
@@ -3068,7 +3071,7 @@
     <row r="8" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q8" s="19" cm="1">
         <f t="array" ref="Q8">Table2[Tagged Today]</f>
-        <v>664</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3730,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4E6563-AFDF-481D-85FD-ACA04DEA8072}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3799,19 +3802,19 @@
       <c r="F2" s="8"/>
       <c r="G2" s="19">
         <f>Total_Tokens - MAX(C2:C13)</f>
-        <v>4579</v>
+        <v>4205</v>
       </c>
       <c r="H2" s="22">
         <f>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</f>
-        <v>0.45266555103992351</v>
+        <v>0.49737030839110685</v>
       </c>
       <c r="I2" s="20">
         <f>G2/COUNTBLANK(C2:C13)</f>
-        <v>457.9</v>
+        <v>467.22222222222223</v>
       </c>
       <c r="J2" s="24" cm="1">
         <f t="array" ref="J2">LOOKUP(2,1/(Table1[Actual Words Tagged]&lt;&gt;""),Table1[Actual Words Tagged])-INDEX(Table1[Actual Words Tagged],MATCH(99^99,Table1[Actual Words Tagged],1)-1)</f>
-        <v>664</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -3844,12 +3847,17 @@
         <f t="shared" si="0"/>
         <v>4076.272727272727</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="20">
+        <v>4161</v>
+      </c>
       <c r="D4" s="20">
         <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
         <v>4289.727272727273</v>
       </c>
-      <c r="E4" s="20"/>
+      <c r="E4" s="20">
+        <f>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</f>
+        <v>4205</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="6"/>
       <c r="H4" s="23"/>

</xml_diff>

<commit_message>
Update Nuuchahnulth data progress.xlsx
</commit_message>
<xml_diff>
--- a/data/reports/Nuuchahnulth data progress.xlsx
+++ b/data/reports/Nuuchahnulth data progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/data/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="839" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{472DD741-7A8D-4EAF-993B-05A9CC051ED3}"/>
+  <xr:revisionPtr revIDLastSave="840" documentId="114_{6660E208-4B16-481A-ABD5-F0BCABA587CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B883328D-CE3B-4AD7-B1E7-3D79FE99CE65}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
   </bookViews>
@@ -793,7 +793,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.55761415252211333</c:v>
+                  <c:v>0.62861582596222809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,7 +1251,7 @@
                   <c:v>4579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3701</c:v>
+                  <c:v>3107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3049,7 +3049,7 @@
     <row r="2" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q2" s="19">
         <f>Table2[[#This Row],[Tokens Remaining]]</f>
-        <v>3701</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="4" spans="17:17" x14ac:dyDescent="0.45">
@@ -3060,7 +3060,7 @@
     <row r="5" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q5" s="20" cm="1">
         <f t="array" ref="Q5">Table2[Daily Average to Hit]</f>
-        <v>411.22222222222223</v>
+        <v>345.22222222222223</v>
       </c>
     </row>
     <row r="7" spans="17:17" x14ac:dyDescent="0.45">
@@ -3071,7 +3071,7 @@
     <row r="8" spans="17:17" x14ac:dyDescent="0.45">
       <c r="Q8" s="19" cm="1">
         <f t="array" ref="Q8">Table2[Tagged Today]</f>
-        <v>878</v>
+        <v>1472</v>
       </c>
     </row>
   </sheetData>
@@ -3802,19 +3802,19 @@
       <c r="F2" s="8"/>
       <c r="G2" s="19">
         <f>Total_Tokens - MAX(C2:C13)</f>
-        <v>3701</v>
+        <v>3107</v>
       </c>
       <c r="H2" s="22">
         <f>(Total_Tokens-Table2[[#This Row],[Tokens Remaining]])/Total_Tokens</f>
-        <v>0.55761415252211333</v>
+        <v>0.62861582596222809</v>
       </c>
       <c r="I2" s="20">
         <f>G2/COUNTBLANK(C2:C13)</f>
-        <v>411.22222222222223</v>
+        <v>345.22222222222223</v>
       </c>
       <c r="J2" s="24" cm="1">
         <f t="array" ref="J2">LOOKUP(2,1/(Table1[Actual Words Tagged]&lt;&gt;""),Table1[Actual Words Tagged])-INDEX(Table1[Actual Words Tagged],MATCH(99^99,Table1[Actual Words Tagged],1)-1)</f>
-        <v>878</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -3848,7 +3848,7 @@
         <v>4076.272727272727</v>
       </c>
       <c r="C4" s="20">
-        <v>4665</v>
+        <v>5259</v>
       </c>
       <c r="D4" s="20">
         <f>Total_Tokens-Table1[[#This Row],[Target Words Tagged]]</f>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="E4" s="20">
         <f>Total_Tokens-Table1[[#This Row],[Actual Words Tagged]]</f>
-        <v>3701</v>
+        <v>3107</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="6"/>

</xml_diff>